<commit_message>
autocolumn when first row of range > 9
</commit_message>
<xml_diff>
--- a/examples/cisco_ios.xlsx
+++ b/examples/cisco_ios.xlsx
@@ -822,12 +822,6 @@
     <t>GigabitEthernet2/0/8</t>
   </si>
   <si>
-    <t>Port Mode</t>
-  </si>
-  <si>
-    <t>VLAN(s)</t>
-  </si>
-  <si>
     <t>GigabitEthernet1/0/9</t>
   </si>
   <si>
@@ -1101,12 +1095,6 @@
     <t>ethernet 1/41</t>
   </si>
   <si>
-    <t>device b</t>
-  </si>
-  <si>
-    <t>device b port</t>
-  </si>
-  <si>
     <t>528</t>
   </si>
   <si>
@@ -1138,6 +1126,18 @@
   </si>
   <si>
     <t>ACMEME1MGT01</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>vlans</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>device_port</t>
   </si>
 </sst>
 </file>
@@ -2467,8 +2467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2500,13 +2500,13 @@
         <v>65</v>
       </c>
       <c r="B2" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>341</v>
-      </c>
       <c r="D2" s="15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2514,10 +2514,10 @@
         <v>100</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>28</v>
@@ -2528,10 +2528,10 @@
         <v>101</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>28</v>
@@ -2542,10 +2542,10 @@
         <v>102</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>28</v>
@@ -2556,10 +2556,10 @@
         <v>103</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>28</v>
@@ -2570,10 +2570,10 @@
         <v>104</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>28</v>
@@ -2584,10 +2584,10 @@
         <v>116</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>28</v>
@@ -2598,10 +2598,10 @@
         <v>117</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>28</v>
@@ -2612,10 +2612,10 @@
         <v>118</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>28</v>
@@ -2626,10 +2626,10 @@
         <v>132</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>28</v>
@@ -2640,10 +2640,10 @@
         <v>148</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>28</v>
@@ -2654,10 +2654,10 @@
         <v>149</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>28</v>
@@ -2671,10 +2671,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2685,7 +2685,7 @@
         <v>232</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>25</v>
@@ -2699,7 +2699,7 @@
         <v>233</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>25</v>
@@ -2713,7 +2713,7 @@
         <v>27</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>25</v>
@@ -2727,7 +2727,7 @@
         <v>234</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>25</v>
@@ -2755,7 +2755,7 @@
         <v>235</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>26</v>
@@ -2769,7 +2769,7 @@
         <v>63</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>26</v>
@@ -2780,10 +2780,10 @@
         <v>529</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>26</v>
@@ -2794,10 +2794,10 @@
         <v>530</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>26</v>
@@ -2808,10 +2808,10 @@
         <v>531</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>26</v>
@@ -2822,10 +2822,10 @@
         <v>532</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>26</v>
@@ -2836,10 +2836,10 @@
         <v>533</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>26</v>
@@ -2850,10 +2850,10 @@
         <v>534</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>26</v>
@@ -2864,17 +2864,17 @@
         <v>535</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:6" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>16</v>
       </c>
@@ -2882,33 +2882,33 @@
         <v>5</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>263</v>
+        <v>365</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>247</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>239</v>
@@ -2920,13 +2920,13 @@
         <v>248</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>240</v>
@@ -2938,13 +2938,13 @@
         <v>249</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>241</v>
@@ -2956,13 +2956,13 @@
         <v>250</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>242</v>
@@ -2974,13 +2974,13 @@
         <v>251</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>239</v>
@@ -2992,13 +2992,13 @@
         <v>252</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F41" s="8" t="s">
         <v>240</v>
@@ -3010,13 +3010,13 @@
         <v>253</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F42" s="8" t="s">
         <v>241</v>
@@ -3028,13 +3028,13 @@
         <v>254</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F43" s="8" t="s">
         <v>242</v>
@@ -3043,16 +3043,16 @@
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="19"/>
       <c r="B44" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>17</v>
@@ -3061,16 +3061,16 @@
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="19"/>
       <c r="B45" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F45" s="8" t="s">
         <v>52</v>
@@ -3079,68 +3079,68 @@
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19"/>
       <c r="B46" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D46" s="8">
         <v>253</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D47" s="8">
         <v>250</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
       <c r="B48" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>238</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="19"/>
       <c r="B49" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>237</v>
@@ -3149,16 +3149,16 @@
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="19"/>
       <c r="B50" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>237</v>
@@ -3167,16 +3167,16 @@
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="19"/>
       <c r="B51" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>237</v>
@@ -3185,16 +3185,16 @@
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19"/>
       <c r="B52" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>237</v>
@@ -3203,16 +3203,16 @@
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19"/>
       <c r="B53" s="6" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F53" s="8" t="s">
         <v>237</v>
@@ -3221,16 +3221,16 @@
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="19"/>
       <c r="B54" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>237</v>
@@ -3239,16 +3239,16 @@
     <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
       <c r="B55" s="6" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>237</v>
@@ -3257,16 +3257,16 @@
     <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19"/>
       <c r="B56" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>237</v>
@@ -3275,16 +3275,16 @@
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19"/>
       <c r="B57" s="6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F57" s="8" t="s">
         <v>237</v>
@@ -3293,16 +3293,16 @@
     <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="19"/>
       <c r="B58" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F58" s="8" t="s">
         <v>237</v>
@@ -3311,16 +3311,16 @@
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F59" s="8" t="s">
         <v>237</v>
@@ -3329,64 +3329,64 @@
     <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="6" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C60" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D60" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>307</v>
-      </c>
       <c r="E60" s="8" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>238</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="19"/>
       <c r="B62" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>238</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19"/>
       <c r="B63" s="6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D63" s="8" t="s">
         <v>238</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F63" s="8"/>
     </row>
@@ -3396,13 +3396,13 @@
         <v>255</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F64" s="8" t="s">
         <v>243</v>
@@ -3414,13 +3414,13 @@
         <v>256</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F65" s="8" t="s">
         <v>244</v>
@@ -3432,13 +3432,13 @@
         <v>257</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F66" s="8" t="s">
         <v>245</v>
@@ -3450,13 +3450,13 @@
         <v>258</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F67" s="8" t="s">
         <v>246</v>
@@ -3468,13 +3468,13 @@
         <v>259</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F68" s="8" t="s">
         <v>243</v>
@@ -3486,13 +3486,13 @@
         <v>260</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E69" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F69" s="8" t="s">
         <v>244</v>
@@ -3504,13 +3504,13 @@
         <v>261</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F70" s="8" t="s">
         <v>245</v>
@@ -3522,13 +3522,13 @@
         <v>262</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F71" s="8" t="s">
         <v>246</v>
@@ -3537,16 +3537,16 @@
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="19"/>
       <c r="B72" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F72" s="8" t="s">
         <v>17</v>
@@ -3555,16 +3555,16 @@
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19"/>
       <c r="B73" s="6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E73" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F73" s="8" t="s">
         <v>19</v>
@@ -3573,34 +3573,34 @@
     <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="19"/>
       <c r="B74" s="6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D74" s="8">
         <v>253</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="19"/>
       <c r="B75" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F75" s="8" t="s">
         <v>17</v>
@@ -3609,49 +3609,49 @@
     <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="19"/>
       <c r="B76" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F76" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="19"/>
       <c r="B77" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="19"/>
       <c r="B78" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F78" s="8" t="s">
         <v>237</v>
@@ -3660,16 +3660,16 @@
     <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="19"/>
       <c r="B79" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F79" s="8" t="s">
         <v>237</v>
@@ -3678,16 +3678,16 @@
     <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="19"/>
       <c r="B80" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F80" s="8" t="s">
         <v>237</v>
@@ -3696,16 +3696,16 @@
     <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="19"/>
       <c r="B81" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>237</v>
@@ -3714,16 +3714,16 @@
     <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="19"/>
       <c r="B82" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F82" s="8" t="s">
         <v>237</v>
@@ -3732,16 +3732,16 @@
     <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="19"/>
       <c r="B83" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F83" s="8" t="s">
         <v>237</v>
@@ -3750,16 +3750,16 @@
     <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="19"/>
       <c r="B84" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F84" s="8" t="s">
         <v>237</v>
@@ -3768,16 +3768,16 @@
     <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="19"/>
       <c r="B85" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>237</v>
@@ -3786,16 +3786,16 @@
     <row r="86" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="19"/>
       <c r="B86" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F86" s="8" t="s">
         <v>237</v>
@@ -3804,16 +3804,16 @@
     <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="19"/>
       <c r="B87" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F87" s="8" t="s">
         <v>237</v>
@@ -3822,66 +3822,66 @@
     <row r="88" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="19"/>
       <c r="B88" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C88" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D88" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D88" s="8" t="s">
-        <v>307</v>
-      </c>
       <c r="E88" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="19"/>
       <c r="B89" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>238</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F89" s="8"/>
     </row>
     <row r="90" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="19"/>
       <c r="B90" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D90" s="8">
         <v>251</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F90" s="8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="20"/>
       <c r="B91" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C91" s="8"/>
       <c r="D91" s="8" t="s">
         <v>238</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F91" s="8"/>
     </row>

</xml_diff>

<commit_message>
modified cisco example. added forcepoint example. populated README.md
</commit_message>
<xml_diff>
--- a/examples/cisco_ios.xlsx
+++ b/examples/cisco_ios.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="370">
   <si>
     <t>Comment</t>
   </si>
@@ -1138,6 +1138,9 @@
   </si>
   <si>
     <t>device_port</t>
+  </si>
+  <si>
+    <t>interface</t>
   </si>
 </sst>
 </file>
@@ -2467,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2879,7 +2882,7 @@
         <v>16</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>5</v>
+        <v>369</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>365</v>

</xml_diff>